<commit_message>
test case created for api and executed for symlex ios
</commit_message>
<xml_diff>
--- a/api/app_api/backlog/remove_user/is_permanent_ delete_negative.xlsx
+++ b/api/app_api/backlog/remove_user/is_permanent_ delete_negative.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\backlog\remove_user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A811CDF-B99C-4C84-AC3B-4C71229DFB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DE646F-35E1-4B40-B2B1-249EBF33C299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login_CRC" sheetId="1" r:id="rId1"/>
+    <sheet name="permanent_delete" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -171,60 +171,20 @@
 Input: 1true</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST)
-4. fill the other required field with valid credentials and goto is permanent delete option
-5. send the request with invalid boolean value "1true"
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>Check with invalid boolean value "0false"
 Input: 0false</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST)
-4. fill the other required field with valid credentials and goto option
-5. send the request with invalid boolean value "0false"
-6. review the response status code.</t>
   </si>
   <si>
     <t>Check with invalid boolean value as a number (2)
 Input: 2</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST)
-4. fill the other required field with valid credentials and goto option
-5. send the request with invalid boolean value as a number (2)
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>Check with invalid boolean value as a string "yes"
 Input: yes</t>
   </si>
   <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST)
-4. fill the other required field with valid credentials and goto option
-5. send the request with invalid boolean value as a string "yes"
-6. review the response status code.</t>
-  </si>
-  <si>
     <t>Check with invalid boolean value as a string "no"
 Input: no</t>
-  </si>
-  <si>
-    <t>1. open the postman
-2. create or open the saved request
-3. define request(method -POST)
-4. fill the other required field with valid credentials and goto option
-5. send the request with invalid boolean value as a string "no"
-6. review the response status code.</t>
   </si>
   <si>
     <t>Check with invalid boolean value as a string containing HTML tags
@@ -356,6 +316,46 @@
 3. define request(method -POST)
 4. fill the other required field with valid credentials and goto is permanent delete option
 5. send the request with invalid boolean value as a string exceeding maximum length
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST)
+4. fill the other required field with valid credentials and goto 'is permanent delete' option
+5. send the request with invalid boolean value "1true"
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST)
+4. fill the other required field with valid credentials and goto 'is permanent delete' option
+5. send the request with invalid boolean value "0false"
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST)
+4. fill the other required field with valid credentials and goto 'is permanent delete' option
+5. send the request with invalid boolean value as a number (2)
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST)
+4. fill the other required field with valid credentials and goto 'is permanent delete' option
+5. send the request with invalid boolean value as a string "yes"
+6. review the response status code.</t>
+  </si>
+  <si>
+    <t>1. open the postman
+2. create or open the saved request
+3. define request(method -POST)
+4. fill the other required field with valid credentials and goto 'is permanent delete' option
+5. send the request with invalid boolean value as a string "no"
 6. review the response status code.</t>
   </si>
 </sst>
@@ -647,11 +647,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -659,49 +655,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -752,6 +707,171 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -785,11 +905,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -797,10 +913,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -861,6 +975,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -878,7 +993,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -887,125 +1006,6 @@
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1568,13 +1568,13 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G7" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" totalsRowLabel="SYM-API-SP-004" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" totalsRowLabel="1. needs to have postman install_x000a_2. needs to have proper defination in the documentation" dataDxfId="12" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" totalsRowLabel="Check with invalid boolean value &quot;falsee&quot;_x000a__x000a_Input: falsee" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" totalsRowLabel="1. open the postman_x000a_2. create or open the saved request_x000a_3. define request(method -POST)_x000a_4. fill the other required field with valid credentials and goto is permanent delete option_x000a_5. send the request with invalid boolean value &quot;falsee&quot;_x000a_6. review the response status code." dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" totalsRowLabel="Post request should fail with status code 400" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" totalsRowLabel="N/A" dataDxfId="8" totalsRowDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" totalsRowLabel="SYM-API-SP-004" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" totalsRowLabel="1. needs to have postman install_x000a_2. needs to have proper defination in the documentation" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" totalsRowLabel="Check with invalid boolean value &quot;falsee&quot;_x000a__x000a_Input: falsee" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" totalsRowLabel="1. open the postman_x000a_2. create or open the saved request_x000a_3. define request(method -POST)_x000a_4. fill the other required field with valid credentials and goto is permanent delete option_x000a_5. send the request with invalid boolean value &quot;falsee&quot;_x000a_6. review the response status code." dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" totalsRowLabel="Post request should fail with status code 400" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" totalsRowLabel="N/A" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1784,8 +1784,8 @@
   <dimension ref="A1:Z963"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2073,7 +2073,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>30</v>
@@ -2110,10 +2110,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>30</v>
@@ -2150,10 +2150,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>30</v>
@@ -2190,10 +2190,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>30</v>
@@ -2230,10 +2230,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>30</v>
@@ -2270,10 +2270,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>30</v>
@@ -2310,10 +2310,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>30</v>
@@ -2350,10 +2350,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>30</v>
@@ -2390,10 +2390,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>30</v>
@@ -2430,10 +2430,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>30</v>
@@ -2470,10 +2470,10 @@
         <v>9</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>30</v>
@@ -2510,10 +2510,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>30</v>
@@ -2550,10 +2550,10 @@
         <v>9</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>30</v>
@@ -2590,10 +2590,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>30</v>
@@ -2630,10 +2630,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>30</v>
@@ -2670,10 +2670,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>30</v>

</xml_diff>